<commit_message>
created public add sheet method
</commit_message>
<xml_diff>
--- a/Test Open Xml/testdata/testaddsheet.xlsx
+++ b/Test Open Xml/testdata/testaddsheet.xlsx
@@ -2,8 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R1542aca031334f0c"/>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B4" sheetId="2" r:id="Rac91988fa1d54790"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R28aaa9f20c37491e"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet4" sheetId="2" r:id="R1dc225bd044c4120"/>
   </x:sheets>
 </x:workbook>
 </file>

</xml_diff>

<commit_message>
improved cell format capability
</commit_message>
<xml_diff>
--- a/Test Open Xml/testdata/testaddsheet.xlsx
+++ b/Test Open Xml/testdata/testaddsheet.xlsx
@@ -2,8 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R28aaa9f20c37491e"/>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet4" sheetId="2" r:id="R1dc225bd044c4120"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R6da328affbaa4d60"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet4" sheetId="2" r:id="Rafff207390964d83"/>
   </x:sheets>
 </x:workbook>
 </file>

</xml_diff>

<commit_message>
basic cell manipulation working
</commit_message>
<xml_diff>
--- a/Test Open Xml/testdata/testaddsheet.xlsx
+++ b/Test Open Xml/testdata/testaddsheet.xlsx
@@ -2,10 +2,32 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R6da328affbaa4d60"/>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet4" sheetId="2" r:id="Rafff207390964d83"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R44088e9b28f2413d"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet4" sheetId="2" r:id="R9ecef7554f8d44d4"/>
   </x:sheets>
 </x:workbook>
+</file>
+
+<file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
+<x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:fonts count="1">
+    <x:font/>
+  </x:fonts>
+  <x:fills count="2">
+    <x:fill>
+      <x:patternFill patternType="none"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="gray125"/>
+    </x:fill>
+  </x:fills>
+  <x:borders count="1">
+    <x:border/>
+  </x:borders>
+  <x:cellXfs count="1">
+    <x:xf/>
+  </x:cellXfs>
+</x:styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
closed some reference leaks
</commit_message>
<xml_diff>
--- a/Test Open Xml/testdata/testaddsheet.xlsx
+++ b/Test Open Xml/testdata/testaddsheet.xlsx
@@ -2,8 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rfd1facbfd22145f8"/>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet4" sheetId="2" r:id="R92985b88d35f4e84"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rbe6577842d1c4bd9"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet4" sheetId="2" r:id="R54e769a90ed34186"/>
   </x:sheets>
 </x:workbook>
 </file>

</xml_diff>

<commit_message>
fixed set/get named range
</commit_message>
<xml_diff>
--- a/Test Open Xml/testdata/testaddsheet.xlsx
+++ b/Test Open Xml/testdata/testaddsheet.xlsx
@@ -2,8 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rbe6577842d1c4bd9"/>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet4" sheetId="2" r:id="R54e769a90ed34186"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R5a9607030825406d"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet4" sheetId="2" r:id="R13318db018bb47d6"/>
   </x:sheets>
 </x:workbook>
 </file>

</xml_diff>

<commit_message>
fixed named range tests
</commit_message>
<xml_diff>
--- a/Test Open Xml/testdata/testaddsheet.xlsx
+++ b/Test Open Xml/testdata/testaddsheet.xlsx
@@ -2,8 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R5a9607030825406d"/>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet4" sheetId="2" r:id="R13318db018bb47d6"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R9475c9bd288e4800"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet4" sheetId="2" r:id="Rdf3b991f0b674421"/>
   </x:sheets>
 </x:workbook>
 </file>

</xml_diff>